<commit_message>
1999 Property Crimes updates
</commit_message>
<xml_diff>
--- a/1999/summary-of-offenses-ibr-agencies-property-crimes-1999.xlsx
+++ b/1999/summary-of-offenses-ibr-agencies-property-crimes-1999.xlsx
@@ -114,9 +114,54 @@
     <t>Sunday</t>
   </si>
   <si>
+    <t>Days of Week/Number of Offenses</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Bribery</t>
+  </si>
+  <si>
+    <t>Counterfeiting/Forgery</t>
+  </si>
+  <si>
+    <t>Destruction/Vandalism</t>
+  </si>
+  <si>
+    <t>Embezzlement</t>
+  </si>
+  <si>
+    <t>Extortion</t>
+  </si>
+  <si>
+    <t>Fraud</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
+    <t>Stolen Property</t>
+  </si>
+  <si>
     <t>Bribery</t>
   </si>
   <si>
@@ -217,54 +262,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Location of offense for arson, larceny, motor vehicle theft, and robbery can be found in the sections pertaining to these individual offenses.</t>
-  </si>
-  <si>
-    <t>Days of Week/Number of Offenses</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Bribery</t>
-  </si>
-  <si>
-    <t>Counterfeiting/Forgery</t>
-  </si>
-  <si>
-    <t>Destruction/Vandalism</t>
-  </si>
-  <si>
-    <t>Embezzlement</t>
-  </si>
-  <si>
-    <t>Extortion</t>
-  </si>
-  <si>
-    <t>Fraud</t>
-  </si>
-  <si>
-    <t>Stolen Property</t>
   </si>
   <si>
     <t>Resident Status of Victims</t>
@@ -366,27 +363,27 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -828,7 +825,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="33.57"/>
+    <col min="1" customWidth="1" max="1" width="31.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -856,182 +853,140 @@
       <c t="s" s="1" r="H1">
         <v>39</v>
       </c>
-      <c t="s" s="1" r="I1">
-        <v>40</v>
-      </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c s="1" r="B2">
         <v>0.0</v>
       </c>
       <c s="1" r="C2">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="D2">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="E2">
-        <v>43.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="F2">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="G2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="H2">
-        <v>18.0</v>
-      </c>
-      <c s="1" r="I2">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c s="1" r="B3">
-        <v>0.0</v>
+        <v>746.0</v>
       </c>
       <c s="1" r="C3">
-        <v>10.0</v>
+        <v>707.0</v>
       </c>
       <c s="1" r="D3">
-        <v>831.0</v>
+        <v>733.0</v>
       </c>
       <c s="1" r="E3">
-        <v>75.0</v>
+        <v>760.0</v>
       </c>
       <c s="1" r="F3">
-        <v>31.0</v>
+        <v>895.0</v>
       </c>
       <c s="1" r="G3">
-        <v>0.0</v>
+        <v>604.0</v>
       </c>
       <c s="1" r="H3">
-        <v>308.0</v>
-      </c>
-      <c s="1" r="I3">
-        <v>4.0</v>
+        <v>458.0</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c s="1" r="B4">
-        <v>0.0</v>
+        <v>6734.0</v>
       </c>
       <c s="1" r="C4">
-        <v>39.0</v>
+        <v>6370.0</v>
       </c>
       <c s="1" r="D4">
-        <v>34.0</v>
+        <v>6262.0</v>
       </c>
       <c s="1" r="E4">
-        <v>143.0</v>
+        <v>6381.0</v>
       </c>
       <c s="1" r="F4">
-        <v>3.0</v>
+        <v>7876.0</v>
       </c>
       <c s="1" r="G4">
-        <v>0.0</v>
+        <v>7842.0</v>
       </c>
       <c s="1" r="H4">
-        <v>31.0</v>
-      </c>
-      <c s="1" r="I4">
-        <v>0.0</v>
+        <v>6993.0</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c s="1" r="B5">
-        <v>0.0</v>
+        <v>199.0</v>
       </c>
       <c s="1" r="C5">
-        <v>227.0</v>
+        <v>165.0</v>
       </c>
       <c s="1" r="D5">
-        <v>4.0</v>
+        <v>180.0</v>
       </c>
       <c s="1" r="E5">
-        <v>389.0</v>
+        <v>170.0</v>
       </c>
       <c s="1" r="F5">
-        <v>2.0</v>
+        <v>229.0</v>
       </c>
       <c s="1" r="G5">
-        <v>0.0</v>
+        <v>159.0</v>
       </c>
       <c s="1" r="H5">
-        <v>7.0</v>
-      </c>
-      <c s="1" r="I5">
-        <v>1.0</v>
+        <v>106.0</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>45</v>
-      </c>
-      <c s="1" r="B6">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C6">
-        <v>832.0</v>
-      </c>
-      <c s="1" r="D6">
-        <v>109.0</v>
-      </c>
-      <c s="1" r="E6">
-        <v>1435.0</v>
-      </c>
-      <c s="1" r="F6">
-        <v>92.0</v>
-      </c>
-      <c s="1" r="G6">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H6">
-        <v>143.0</v>
-      </c>
-      <c s="1" r="I6">
-        <v>8.0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c s="1" r="B7">
-        <v>0.0</v>
+        <v>728.0</v>
       </c>
       <c s="1" r="C7">
-        <v>277.0</v>
+        <v>687.0</v>
       </c>
       <c s="1" r="D7">
-        <v>4.0</v>
+        <v>613.0</v>
       </c>
       <c s="1" r="E7">
-        <v>624.0</v>
+        <v>674.0</v>
       </c>
       <c s="1" r="F7">
-        <v>3.0</v>
+        <v>718.0</v>
       </c>
       <c s="1" r="G7">
-        <v>0.0</v>
+        <v>593.0</v>
       </c>
       <c s="1" r="H7">
-        <v>12.0</v>
-      </c>
-      <c s="1" r="I7">
-        <v>2.0</v>
+        <v>384.0</v>
       </c>
     </row>
     <row r="8">
@@ -1039,588 +994,26 @@
         <v>47</v>
       </c>
       <c s="1" r="B8">
-        <v>0.0</v>
+        <v>107.0</v>
       </c>
       <c s="1" r="C8">
-        <v>331.0</v>
+        <v>93.0</v>
       </c>
       <c s="1" r="D8">
-        <v>618.0</v>
+        <v>101.0</v>
       </c>
       <c s="1" r="E8">
-        <v>553.0</v>
+        <v>89.0</v>
       </c>
       <c s="1" r="F8">
-        <v>94.0</v>
+        <v>105.0</v>
       </c>
       <c s="1" r="G8">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c s="1" r="H8">
-        <v>230.0</v>
-      </c>
-      <c s="1" r="I8">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>48</v>
-      </c>
-      <c s="1" r="B9">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C9">
-        <v>125.0</v>
-      </c>
-      <c s="1" r="D9">
-        <v>370.0</v>
-      </c>
-      <c s="1" r="E9">
-        <v>313.0</v>
-      </c>
-      <c s="1" r="F9">
-        <v>330.0</v>
-      </c>
-      <c s="1" r="G9">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H9">
-        <v>489.0</v>
-      </c>
-      <c s="1" r="I9">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>49</v>
-      </c>
-      <c s="1" r="B10">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C10">
-        <v>90.0</v>
-      </c>
-      <c s="1" r="D10">
-        <v>178.0</v>
-      </c>
-      <c s="1" r="E10">
-        <v>183.0</v>
-      </c>
-      <c s="1" r="F10">
-        <v>20.0</v>
-      </c>
-      <c s="1" r="G10">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H10">
-        <v>171.0</v>
-      </c>
-      <c s="1" r="I10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>50</v>
-      </c>
-      <c s="1" r="B11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C11">
-        <v>11.0</v>
-      </c>
-      <c s="1" r="D11">
-        <v>9.0</v>
-      </c>
-      <c s="1" r="E11">
-        <v>499.0</v>
-      </c>
-      <c s="1" r="F11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="G11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H11">
-        <v>5.0</v>
-      </c>
-      <c s="1" r="I11">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>51</v>
-      </c>
-      <c s="1" r="B12">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C12">
-        <v>148.0</v>
-      </c>
-      <c s="1" r="D12">
-        <v>114.0</v>
-      </c>
-      <c s="1" r="E12">
-        <v>516.0</v>
-      </c>
-      <c s="1" r="F12">
-        <v>7.0</v>
-      </c>
-      <c s="1" r="G12">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H12">
-        <v>43.0</v>
-      </c>
-      <c s="1" r="I12">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>52</v>
-      </c>
-      <c s="1" r="B13">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C13">
-        <v>111.0</v>
-      </c>
-      <c s="1" r="D13">
-        <v>812.0</v>
-      </c>
-      <c s="1" r="E13">
-        <v>242.0</v>
-      </c>
-      <c s="1" r="F13">
-        <v>68.0</v>
-      </c>
-      <c s="1" r="G13">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H13">
-        <v>346.0</v>
-      </c>
-      <c s="1" r="I13">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>53</v>
-      </c>
-      <c s="1" r="B14">
-        <v>4.0</v>
-      </c>
-      <c s="1" r="C14">
-        <v>16.0</v>
-      </c>
-      <c s="1" r="D14">
-        <v>318.0</v>
-      </c>
-      <c s="1" r="E14">
-        <v>6563.0</v>
-      </c>
-      <c s="1" r="F14">
-        <v>1.0</v>
-      </c>
-      <c s="1" r="G14">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H14">
-        <v>140.0</v>
-      </c>
-      <c s="1" r="I14">
-        <v>244.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
-        <v>54</v>
-      </c>
-      <c s="1" r="B15">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C15">
-        <v>139.0</v>
-      </c>
-      <c s="1" r="D15">
-        <v>21.0</v>
-      </c>
-      <c s="1" r="E15">
-        <v>448.0</v>
-      </c>
-      <c s="1" r="F15">
-        <v>23.0</v>
-      </c>
-      <c s="1" r="G15">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H15">
-        <v>95.0</v>
-      </c>
-      <c s="1" r="I15">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
-        <v>55</v>
-      </c>
-      <c s="1" r="B16">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C16">
-        <v>3.0</v>
-      </c>
-      <c s="1" r="D16">
-        <v>84.0</v>
-      </c>
-      <c s="1" r="E16">
-        <v>48.0</v>
-      </c>
-      <c s="1" r="F16">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="G16">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H16">
-        <v>7.0</v>
-      </c>
-      <c s="1" r="I16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>56</v>
-      </c>
-      <c s="1" r="B17">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C17">
-        <v>11.0</v>
-      </c>
-      <c s="1" r="D17">
-        <v>1.0</v>
-      </c>
-      <c s="1" r="E17">
-        <v>49.0</v>
-      </c>
-      <c s="1" r="F17">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="G17">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H17">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I17">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>57</v>
-      </c>
-      <c s="1" r="B18">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C18">
-        <v>7.0</v>
-      </c>
-      <c s="1" r="D18">
-        <v>4.0</v>
-      </c>
-      <c s="1" r="E18">
-        <v>12.0</v>
-      </c>
-      <c s="1" r="F18">
-        <v>1.0</v>
-      </c>
-      <c s="1" r="G18">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H18">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I18">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>58</v>
-      </c>
-      <c s="1" r="B19">
-        <v>1.0</v>
-      </c>
-      <c s="1" r="C19">
-        <v>208.0</v>
-      </c>
-      <c s="1" r="D19">
-        <v>39.0</v>
-      </c>
-      <c s="1" r="E19">
-        <v>7840.0</v>
-      </c>
-      <c s="1" r="F19">
-        <v>4.0</v>
-      </c>
-      <c s="1" r="G19">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H19">
-        <v>80.0</v>
-      </c>
-      <c s="1" r="I19">
-        <v>84.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>59</v>
-      </c>
-      <c s="1" r="B20">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C20">
-        <v>188.0</v>
-      </c>
-      <c s="1" r="D20">
-        <v>2.0</v>
-      </c>
-      <c s="1" r="E20">
-        <v>211.0</v>
-      </c>
-      <c s="1" r="F20">
-        <v>9.0</v>
-      </c>
-      <c s="1" r="G20">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H20">
-        <v>44.0</v>
-      </c>
-      <c s="1" r="I20">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>60</v>
-      </c>
-      <c s="1" r="B21">
-        <v>4.0</v>
-      </c>
-      <c s="1" r="C21">
-        <v>11951.0</v>
-      </c>
-      <c s="1" r="D21">
-        <v>412.0</v>
-      </c>
-      <c s="1" r="E21">
-        <v>21860.0</v>
-      </c>
-      <c s="1" r="F21">
-        <v>43.0</v>
-      </c>
-      <c s="1" r="G21">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H21">
-        <v>932.0</v>
-      </c>
-      <c s="1" r="I21">
-        <v>153.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>61</v>
-      </c>
-      <c s="1" r="B22">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C22">
-        <v>335.0</v>
-      </c>
-      <c s="1" r="D22">
-        <v>197.0</v>
-      </c>
-      <c s="1" r="E22">
-        <v>553.0</v>
-      </c>
-      <c s="1" r="F22">
-        <v>176.0</v>
-      </c>
-      <c s="1" r="G22">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H22">
-        <v>163.0</v>
-      </c>
-      <c s="1" r="I22">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>62</v>
-      </c>
-      <c s="1" r="B23">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C23">
-        <v>368.0</v>
-      </c>
-      <c s="1" r="D23">
-        <v>43.0</v>
-      </c>
-      <c s="1" r="E23">
-        <v>2171.0</v>
-      </c>
-      <c s="1" r="F23">
-        <v>16.0</v>
-      </c>
-      <c s="1" r="G23">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H23">
-        <v>39.0</v>
-      </c>
-      <c s="1" r="I23">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>63</v>
-      </c>
-      <c s="1" r="B24">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C24">
-        <v>154.0</v>
-      </c>
-      <c s="1" r="D24">
-        <v>141.0</v>
-      </c>
-      <c s="1" r="E24">
-        <v>434.0</v>
-      </c>
-      <c s="1" r="F24">
-        <v>41.0</v>
-      </c>
-      <c s="1" r="G24">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H24">
-        <v>176.0</v>
-      </c>
-      <c s="1" r="I24">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>64</v>
-      </c>
-      <c s="1" r="B25">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="C25">
-        <v>653.0</v>
-      </c>
-      <c s="1" r="D25">
-        <v>204.0</v>
-      </c>
-      <c s="1" r="E25">
-        <v>771.0</v>
-      </c>
-      <c s="1" r="F25">
-        <v>143.0</v>
-      </c>
-      <c s="1" r="G25">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H25">
-        <v>402.0</v>
-      </c>
-      <c s="1" r="I25">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>65</v>
-      </c>
-      <c s="1" r="B26">
-        <v>4.0</v>
-      </c>
-      <c s="1" r="C26">
-        <v>855.0</v>
-      </c>
-      <c s="1" r="D26">
-        <v>345.0</v>
-      </c>
-      <c s="1" r="E26">
-        <v>2483.0</v>
-      </c>
-      <c s="1" r="F26">
-        <v>90.0</v>
-      </c>
-      <c s="1" r="G26">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H26">
-        <v>516.0</v>
-      </c>
-      <c s="1" r="I26">
-        <v>65.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>66</v>
-      </c>
-      <c s="1" r="B27">
-        <v>13.0</v>
-      </c>
-      <c s="1" r="C27">
-        <v>17112.0</v>
-      </c>
-      <c s="1" r="D27">
-        <v>4903.0</v>
-      </c>
-      <c s="1" r="E27">
-        <v>48458.0</v>
-      </c>
-      <c s="1" r="F27">
-        <v>1208.0</v>
-      </c>
-      <c s="1" r="G27">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H27">
-        <v>4397.0</v>
-      </c>
-      <c s="1" r="I27">
-        <v>684.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29">
-      <c s="1" r="A29"/>
+        <v>89.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1634,195 +1027,794 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="31.57"/>
+    <col min="1" customWidth="1" max="1" width="33.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c t="s" s="1" r="C1">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="D1">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c t="s" s="1" r="E1">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c t="s" s="1" r="F1">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="G1">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c t="s" s="1" r="H1">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c s="1" r="B2">
         <v>0.0</v>
       </c>
       <c s="1" r="C2">
-        <v>3.0</v>
+        <v>23.0</v>
       </c>
       <c s="1" r="D2">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c s="1" r="E2">
-        <v>5.0</v>
+        <v>43.0</v>
       </c>
       <c s="1" r="F2">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c s="1" r="G2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H2">
-        <v>2.0</v>
+        <v>18.0</v>
+      </c>
+      <c s="1" r="I2">
+        <v>9.0</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c s="1" r="B3">
-        <v>746.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="C3">
-        <v>707.0</v>
+        <v>10.0</v>
       </c>
       <c s="1" r="D3">
-        <v>733.0</v>
+        <v>831.0</v>
       </c>
       <c s="1" r="E3">
-        <v>760.0</v>
+        <v>75.0</v>
       </c>
       <c s="1" r="F3">
-        <v>895.0</v>
+        <v>31.0</v>
       </c>
       <c s="1" r="G3">
-        <v>604.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H3">
-        <v>458.0</v>
+        <v>308.0</v>
+      </c>
+      <c s="1" r="I3">
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c s="1" r="B4">
-        <v>6734.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="C4">
-        <v>6370.0</v>
+        <v>39.0</v>
       </c>
       <c s="1" r="D4">
-        <v>6262.0</v>
+        <v>34.0</v>
       </c>
       <c s="1" r="E4">
-        <v>6381.0</v>
+        <v>143.0</v>
       </c>
       <c s="1" r="F4">
-        <v>7876.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="G4">
-        <v>7842.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H4">
-        <v>6993.0</v>
+        <v>31.0</v>
+      </c>
+      <c s="1" r="I4">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c s="1" r="B5">
-        <v>199.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="C5">
-        <v>165.0</v>
+        <v>227.0</v>
       </c>
       <c s="1" r="D5">
-        <v>180.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="E5">
-        <v>170.0</v>
+        <v>389.0</v>
       </c>
       <c s="1" r="F5">
-        <v>229.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="G5">
-        <v>159.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H5">
-        <v>106.0</v>
+        <v>7.0</v>
+      </c>
+      <c s="1" r="I5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c s="1" r="B6">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C6">
+        <v>832.0</v>
+      </c>
+      <c s="1" r="D6">
+        <v>109.0</v>
+      </c>
+      <c s="1" r="E6">
+        <v>1435.0</v>
+      </c>
+      <c s="1" r="F6">
+        <v>92.0</v>
+      </c>
+      <c s="1" r="G6">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H6">
+        <v>143.0</v>
+      </c>
+      <c s="1" r="I6">
+        <v>8.0</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c s="1" r="B7">
-        <v>728.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="C7">
-        <v>687.0</v>
+        <v>277.0</v>
       </c>
       <c s="1" r="D7">
-        <v>613.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="E7">
-        <v>674.0</v>
+        <v>624.0</v>
       </c>
       <c s="1" r="F7">
-        <v>718.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="G7">
-        <v>593.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H7">
-        <v>384.0</v>
+        <v>12.0</v>
+      </c>
+      <c s="1" r="I7">
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c s="1" r="B8">
-        <v>107.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="C8">
-        <v>93.0</v>
+        <v>331.0</v>
       </c>
       <c s="1" r="D8">
-        <v>101.0</v>
+        <v>618.0</v>
       </c>
       <c s="1" r="E8">
-        <v>89.0</v>
+        <v>553.0</v>
       </c>
       <c s="1" r="F8">
-        <v>105.0</v>
+        <v>94.0</v>
       </c>
       <c s="1" r="G8">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H8">
-        <v>89.0</v>
-      </c>
+        <v>230.0</v>
+      </c>
+      <c s="1" r="I8">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>63</v>
+      </c>
+      <c s="1" r="B9">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C9">
+        <v>125.0</v>
+      </c>
+      <c s="1" r="D9">
+        <v>370.0</v>
+      </c>
+      <c s="1" r="E9">
+        <v>313.0</v>
+      </c>
+      <c s="1" r="F9">
+        <v>330.0</v>
+      </c>
+      <c s="1" r="G9">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H9">
+        <v>489.0</v>
+      </c>
+      <c s="1" r="I9">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>64</v>
+      </c>
+      <c s="1" r="B10">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C10">
+        <v>90.0</v>
+      </c>
+      <c s="1" r="D10">
+        <v>178.0</v>
+      </c>
+      <c s="1" r="E10">
+        <v>183.0</v>
+      </c>
+      <c s="1" r="F10">
+        <v>20.0</v>
+      </c>
+      <c s="1" r="G10">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H10">
+        <v>171.0</v>
+      </c>
+      <c s="1" r="I10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>65</v>
+      </c>
+      <c s="1" r="B11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C11">
+        <v>11.0</v>
+      </c>
+      <c s="1" r="D11">
+        <v>9.0</v>
+      </c>
+      <c s="1" r="E11">
+        <v>499.0</v>
+      </c>
+      <c s="1" r="F11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="G11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H11">
+        <v>5.0</v>
+      </c>
+      <c s="1" r="I11">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>66</v>
+      </c>
+      <c s="1" r="B12">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C12">
+        <v>148.0</v>
+      </c>
+      <c s="1" r="D12">
+        <v>114.0</v>
+      </c>
+      <c s="1" r="E12">
+        <v>516.0</v>
+      </c>
+      <c s="1" r="F12">
+        <v>7.0</v>
+      </c>
+      <c s="1" r="G12">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H12">
+        <v>43.0</v>
+      </c>
+      <c s="1" r="I12">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>67</v>
+      </c>
+      <c s="1" r="B13">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C13">
+        <v>111.0</v>
+      </c>
+      <c s="1" r="D13">
+        <v>812.0</v>
+      </c>
+      <c s="1" r="E13">
+        <v>242.0</v>
+      </c>
+      <c s="1" r="F13">
+        <v>68.0</v>
+      </c>
+      <c s="1" r="G13">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H13">
+        <v>346.0</v>
+      </c>
+      <c s="1" r="I13">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>68</v>
+      </c>
+      <c s="1" r="B14">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="C14">
+        <v>16.0</v>
+      </c>
+      <c s="1" r="D14">
+        <v>318.0</v>
+      </c>
+      <c s="1" r="E14">
+        <v>6563.0</v>
+      </c>
+      <c s="1" r="F14">
+        <v>1.0</v>
+      </c>
+      <c s="1" r="G14">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H14">
+        <v>140.0</v>
+      </c>
+      <c s="1" r="I14">
+        <v>244.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>69</v>
+      </c>
+      <c s="1" r="B15">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C15">
+        <v>139.0</v>
+      </c>
+      <c s="1" r="D15">
+        <v>21.0</v>
+      </c>
+      <c s="1" r="E15">
+        <v>448.0</v>
+      </c>
+      <c s="1" r="F15">
+        <v>23.0</v>
+      </c>
+      <c s="1" r="G15">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H15">
+        <v>95.0</v>
+      </c>
+      <c s="1" r="I15">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>70</v>
+      </c>
+      <c s="1" r="B16">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C16">
+        <v>3.0</v>
+      </c>
+      <c s="1" r="D16">
+        <v>84.0</v>
+      </c>
+      <c s="1" r="E16">
+        <v>48.0</v>
+      </c>
+      <c s="1" r="F16">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="G16">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H16">
+        <v>7.0</v>
+      </c>
+      <c s="1" r="I16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>71</v>
+      </c>
+      <c s="1" r="B17">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C17">
+        <v>11.0</v>
+      </c>
+      <c s="1" r="D17">
+        <v>1.0</v>
+      </c>
+      <c s="1" r="E17">
+        <v>49.0</v>
+      </c>
+      <c s="1" r="F17">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="G17">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H17">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I17">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>72</v>
+      </c>
+      <c s="1" r="B18">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C18">
+        <v>7.0</v>
+      </c>
+      <c s="1" r="D18">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="E18">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="F18">
+        <v>1.0</v>
+      </c>
+      <c s="1" r="G18">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H18">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>73</v>
+      </c>
+      <c s="1" r="B19">
+        <v>1.0</v>
+      </c>
+      <c s="1" r="C19">
+        <v>208.0</v>
+      </c>
+      <c s="1" r="D19">
+        <v>39.0</v>
+      </c>
+      <c s="1" r="E19">
+        <v>7840.0</v>
+      </c>
+      <c s="1" r="F19">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="G19">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H19">
+        <v>80.0</v>
+      </c>
+      <c s="1" r="I19">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>74</v>
+      </c>
+      <c s="1" r="B20">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C20">
+        <v>188.0</v>
+      </c>
+      <c s="1" r="D20">
+        <v>2.0</v>
+      </c>
+      <c s="1" r="E20">
+        <v>211.0</v>
+      </c>
+      <c s="1" r="F20">
+        <v>9.0</v>
+      </c>
+      <c s="1" r="G20">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H20">
+        <v>44.0</v>
+      </c>
+      <c s="1" r="I20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>75</v>
+      </c>
+      <c s="1" r="B21">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="C21">
+        <v>11951.0</v>
+      </c>
+      <c s="1" r="D21">
+        <v>412.0</v>
+      </c>
+      <c s="1" r="E21">
+        <v>21860.0</v>
+      </c>
+      <c s="1" r="F21">
+        <v>43.0</v>
+      </c>
+      <c s="1" r="G21">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H21">
+        <v>932.0</v>
+      </c>
+      <c s="1" r="I21">
+        <v>153.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>76</v>
+      </c>
+      <c s="1" r="B22">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C22">
+        <v>335.0</v>
+      </c>
+      <c s="1" r="D22">
+        <v>197.0</v>
+      </c>
+      <c s="1" r="E22">
+        <v>553.0</v>
+      </c>
+      <c s="1" r="F22">
+        <v>176.0</v>
+      </c>
+      <c s="1" r="G22">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H22">
+        <v>163.0</v>
+      </c>
+      <c s="1" r="I22">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>77</v>
+      </c>
+      <c s="1" r="B23">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C23">
+        <v>368.0</v>
+      </c>
+      <c s="1" r="D23">
+        <v>43.0</v>
+      </c>
+      <c s="1" r="E23">
+        <v>2171.0</v>
+      </c>
+      <c s="1" r="F23">
+        <v>16.0</v>
+      </c>
+      <c s="1" r="G23">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H23">
+        <v>39.0</v>
+      </c>
+      <c s="1" r="I23">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>78</v>
+      </c>
+      <c s="1" r="B24">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C24">
+        <v>154.0</v>
+      </c>
+      <c s="1" r="D24">
+        <v>141.0</v>
+      </c>
+      <c s="1" r="E24">
+        <v>434.0</v>
+      </c>
+      <c s="1" r="F24">
+        <v>41.0</v>
+      </c>
+      <c s="1" r="G24">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H24">
+        <v>176.0</v>
+      </c>
+      <c s="1" r="I24">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>79</v>
+      </c>
+      <c s="1" r="B25">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="C25">
+        <v>653.0</v>
+      </c>
+      <c s="1" r="D25">
+        <v>204.0</v>
+      </c>
+      <c s="1" r="E25">
+        <v>771.0</v>
+      </c>
+      <c s="1" r="F25">
+        <v>143.0</v>
+      </c>
+      <c s="1" r="G25">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H25">
+        <v>402.0</v>
+      </c>
+      <c s="1" r="I25">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>80</v>
+      </c>
+      <c s="1" r="B26">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="C26">
+        <v>855.0</v>
+      </c>
+      <c s="1" r="D26">
+        <v>345.0</v>
+      </c>
+      <c s="1" r="E26">
+        <v>2483.0</v>
+      </c>
+      <c s="1" r="F26">
+        <v>90.0</v>
+      </c>
+      <c s="1" r="G26">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H26">
+        <v>516.0</v>
+      </c>
+      <c s="1" r="I26">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>81</v>
+      </c>
+      <c s="1" r="B27">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="C27">
+        <v>17112.0</v>
+      </c>
+      <c s="1" r="D27">
+        <v>4903.0</v>
+      </c>
+      <c s="1" r="E27">
+        <v>48458.0</v>
+      </c>
+      <c s="1" r="F27">
+        <v>1208.0</v>
+      </c>
+      <c s="1" r="G27">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H27">
+        <v>4397.0</v>
+      </c>
+      <c s="1" r="I27">
+        <v>684.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c s="1" r="A28"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1841,21 +1833,21 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="B1">
         <v>83</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c t="s" s="1" r="C1">
         <v>84</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c t="s" s="1" r="D1">
         <v>85</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c s="1" r="B2">
         <v>77879.0</v>
@@ -1884,24 +1876,24 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="B1">
         <v>88</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c t="s" s="1" r="C1">
         <v>89</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c t="s" s="1" r="D1">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c t="s" s="1" r="E1">
         <v>91</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c s="1" r="B2">
         <v>54021.0</v>
@@ -1918,7 +1910,7 @@
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c s="1" r="B3">
         <v>15472.0</v>
@@ -1935,7 +1927,7 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c s="1" r="B4">
         <v>71.0</v>
@@ -1952,7 +1944,7 @@
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c s="1" r="B5">
         <v>810.0</v>
@@ -1969,7 +1961,7 @@
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c s="1" r="B6">
         <v>2183.0</v>
@@ -1986,7 +1978,7 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c s="1" r="B7">
         <v>72557.0</v>

</xml_diff>